<commit_message>
fix: change invalid data in example xlsx
</commit_message>
<xml_diff>
--- a/public/broker-openapi-example.xlsx
+++ b/public/broker-openapi-example.xlsx
@@ -115,7 +115,7 @@
 }</t>
   </si>
   <si>
-    <t>Ged</t>
+    <t>GET</t>
   </si>
 </sst>
 </file>
@@ -212,14 +212,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -589,10 +589,10 @@
       <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="15"/>
+      <c r="B7" s="17"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
@@ -626,10 +626,10 @@
       <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="15"/>
+      <c r="B10" s="17"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
@@ -640,7 +640,7 @@
       <c r="A11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="17">
+      <c r="B11" s="16">
         <v>200</v>
       </c>
       <c r="C11" s="7"/>
@@ -684,7 +684,7 @@
       <c r="A15" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="16">
+      <c r="B15" s="15">
         <v>201</v>
       </c>
     </row>
@@ -759,7 +759,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -844,10 +844,10 @@
       <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="15"/>
+      <c r="B7" s="17"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
@@ -879,10 +879,10 @@
       <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="15"/>
+      <c r="B10" s="17"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
@@ -893,7 +893,7 @@
       <c r="A11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="17">
+      <c r="B11" s="16">
         <v>200</v>
       </c>
       <c r="C11" s="7"/>

</xml_diff>